<commit_message>
soil N pool and transformation data wrangled, gotten into Tanguro-MasterDataSheet.csv
</commit_message>
<xml_diff>
--- a/Soil-Data-Raw-R/Soil-Data-RawFolders/CN-ratio-percents/LECO CN  Christine Sierra O'Connell   AGOSTO 2013.xlsx
+++ b/Soil-Data-Raw-R/Soil-Data-RawFolders/CN-ratio-percents/LECO CN  Christine Sierra O'Connell   AGOSTO 2013.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25725"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="330" windowWidth="20835" windowHeight="13065"/>
+    <workbookView xWindow="9880" yWindow="5660" windowWidth="20840" windowHeight="13060"/>
   </bookViews>
   <sheets>
     <sheet name="RESULTS" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>CSC S1</t>
   </si>
@@ -95,17 +100,20 @@
   </si>
   <si>
     <t>% Nitrogenio</t>
+  </si>
+  <si>
+    <t>avgs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="167" formatCode="#,##0.000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -118,6 +126,18 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -138,8 +158,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -149,19 +175,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -171,7 +197,13 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -463,19 +495,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -819,10 +851,48 @@
         <v>14.580098800282286</v>
       </c>
     </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="3">
+        <f>AVERAGE(B8:B13)</f>
+        <v>1.6371666666666667</v>
+      </c>
+      <c r="C29" s="3">
+        <f>AVERAGE(C8:C13)</f>
+        <v>0.12441833333333334</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="B30" s="3">
+        <f>AVERAGE(B14:B19)</f>
+        <v>1.6331666666666667</v>
+      </c>
+      <c r="C30" s="3">
+        <f>AVERAGE(C14:C19)</f>
+        <v>0.13056666666666666</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="B31" s="3">
+        <f>AVERAGE(B20:B25)</f>
+        <v>2.153</v>
+      </c>
+      <c r="C31" s="3">
+        <f>AVERAGE(C20:C25)</f>
+        <v>0.13884333333333335</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.49212598499999999" footer="0.49212598499999999"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>